<commit_message>
add transaction functions without appropriate checks yet
</commit_message>
<xml_diff>
--- a/examples/example_transactions.xlsx
+++ b/examples/example_transactions.xlsx
@@ -21,18 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>Narration</t>
-  </si>
-  <si>
     <t>Asset1</t>
   </si>
   <si>
@@ -51,10 +39,22 @@
     <t>sold Asset1 on market</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>bought Asset1 on market</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>narration</t>
   </si>
 </sst>
 </file>
@@ -382,11 +382,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -397,29 +395,29 @@
     <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>42740</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -428,19 +426,15 @@
         <v>1.03</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2">
-        <f>WEEKDAY(A2)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>42743</v>
+        <v>42744</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>-25</v>
@@ -449,15 +443,15 @@
         <v>5.05</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>42747</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -466,15 +460,15 @@
         <v>10.3</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>42750</v>
+        <v>42748</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>-50</v>
@@ -483,7 +477,7 @@
         <v>1.01</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>